<commit_message>
Updated to GTest framework & started Equity work.
Updated to GTest framework & started Equity work.
</commit_message>
<xml_diff>
--- a/Workbooks/Calc_Workspace.xlsx
+++ b/Workbooks/Calc_Workspace.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25035" windowHeight="11715" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25035" windowHeight="11715"/>
   </bookViews>
   <sheets>
-    <sheet name="Simple Interest Rates" sheetId="1" r:id="rId1"/>
-    <sheet name="Cashflows" sheetId="2" r:id="rId2"/>
+    <sheet name="IR, CF, BM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>face</t>
   </si>
@@ -58,15 +57,55 @@
   </si>
   <si>
     <t>Book Example</t>
+  </si>
+  <si>
+    <t>Instutuion</t>
+  </si>
+  <si>
+    <t>Principal</t>
+  </si>
+  <si>
+    <t>Coupon</t>
+  </si>
+  <si>
+    <t>Periods</t>
+  </si>
+  <si>
+    <t>Example 1</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>FV</t>
+  </si>
+  <si>
+    <t>XOM</t>
+  </si>
+  <si>
+    <t>Example 3</t>
+  </si>
+  <si>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>Simple Interest</t>
+  </si>
+  <si>
+    <t>Bond Modeling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.0000_);[Red]\(&quot;$&quot;#,##0.0000\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.0000_);[Red]\(&quot;$&quot;#,##0.0000\)"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -149,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -207,8 +246,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -217,8 +265,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
@@ -233,12 +282,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Explanatory Text" xfId="6" builtinId="53"/>
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="8" builtinId="19"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="3" builtinId="21"/>
@@ -555,267 +636,427 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B2" s="5">
         <v>10000</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B3" s="4">
         <v>4</v>
       </c>
-      <c r="D2" s="1">
-        <f>B1+(B1*B3)</f>
+      <c r="D3" s="1">
+        <f>B2+(B2*B4)</f>
         <v>10500</v>
       </c>
-      <c r="E2" s="1">
-        <f>B1*(POWER(1+B3,B2))</f>
+      <c r="E3" s="1">
+        <f>B2*(POWER(1+B4,B3))</f>
         <v>12155.0625</v>
       </c>
-      <c r="F2" s="1">
-        <f>B1*EXP(B3*B2)</f>
+      <c r="F3" s="1">
+        <f>B2*EXP(B4*B3)</f>
         <v>12214.027581601698</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B4" s="6">
         <v>0.05</v>
       </c>
     </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5">
+        <v>200</v>
+      </c>
+      <c r="C15" s="1">
+        <f>B15/POWER(1+B$12,A15)</f>
+        <v>190.47619047619048</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
+        <v>200</v>
+      </c>
+      <c r="G15" s="1">
+        <f>F15/POWER(1+F$12,E15)</f>
+        <v>185.18518518518516</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <f>A15+1</f>
+        <v>2</v>
+      </c>
+      <c r="B16" s="5">
+        <v>300</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" ref="C16:C18" si="0">B16/POWER(1+B$12,A16)</f>
+        <v>272.10884353741494</v>
+      </c>
+      <c r="E16" s="9">
+        <f>E15+1</f>
+        <v>2</v>
+      </c>
+      <c r="F16" s="5">
+        <v>300</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" ref="G16:G20" si="1">F16/POWER(1+F$12,E16)</f>
+        <v>257.20164609053495</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <f t="shared" ref="A17:A18" si="2">A16+1</f>
+        <v>3</v>
+      </c>
+      <c r="B17" s="5">
+        <v>500</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>431.91879926573802</v>
+      </c>
+      <c r="E17" s="9">
+        <f t="shared" ref="E17:E20" si="3">E16+1</f>
+        <v>3</v>
+      </c>
+      <c r="F17" s="5">
+        <v>500</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>396.9161205100848</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B18" s="5">
+        <v>-1000</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>-822.70247479188197</v>
+      </c>
+      <c r="E18" s="9">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1500</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="1"/>
+        <v>1102.5447791946799</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E19" s="9">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="F19" s="5">
+        <v>600</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="1"/>
+        <v>408.34991822025182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="12">
+        <f>SUM(C15:C18)</f>
+        <v>71.801358487461471</v>
+      </c>
+      <c r="E20" s="9">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F20" s="5">
+        <f>SUM(F15:F19)*-1</f>
+        <v>-3100</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="1"/>
+        <v>-1953.5258433376241</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="12">
+        <f>SUM(G15:G20)</f>
+        <v>396.67180586311247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="15"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="15"/>
+      <c r="G27" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="17">
+        <v>100000</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="17">
+        <v>200000</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="17">
+        <v>190000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="17">
+        <v>5000</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="17">
+        <v>7500</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="17">
+        <v>6589</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="18">
+        <v>30</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="18">
+        <v>20</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="19">
+        <f>B30/B29</f>
+        <v>0.05</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="21">
+        <f>E30/E29</f>
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="22">
+        <f>H30/H29</f>
+        <v>3.4678947368421052E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="20">
+        <f>B29+B30*B31</f>
+        <v>250000</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="20">
+        <f>E29+E30*E31</f>
+        <v>350000</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="20">
+        <f>H29+H30*H31</f>
+        <v>354725</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="E1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="10">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5">
-        <v>200</v>
-      </c>
-      <c r="C5" s="1">
-        <f>B5/POWER(1+B$2,A5)</f>
-        <v>190.47619047619048</v>
-      </c>
-      <c r="E5" s="9">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5">
-        <v>200</v>
-      </c>
-      <c r="G5" s="1">
-        <f>F5/POWER(1+F$2,E5)</f>
-        <v>185.18518518518516</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
-        <f>A5+1</f>
-        <v>2</v>
-      </c>
-      <c r="B6" s="5">
-        <v>300</v>
-      </c>
-      <c r="C6" s="1">
-        <f>B6/POWER(1+B$2,A6)</f>
-        <v>272.10884353741494</v>
-      </c>
-      <c r="E6" s="9">
-        <f>E5+1</f>
-        <v>2</v>
-      </c>
-      <c r="F6" s="5">
-        <v>300</v>
-      </c>
-      <c r="G6" s="1">
-        <f>F6/POWER(1+F$2,E6)</f>
-        <v>257.20164609053495</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <f t="shared" ref="A7:A8" si="0">A6+1</f>
-        <v>3</v>
-      </c>
-      <c r="B7" s="5">
-        <v>500</v>
-      </c>
-      <c r="C7" s="1">
-        <f>B7/POWER(1+B$2,A7)</f>
-        <v>431.91879926573802</v>
-      </c>
-      <c r="E7" s="9">
-        <f t="shared" ref="E7:E10" si="1">E6+1</f>
-        <v>3</v>
-      </c>
-      <c r="F7" s="5">
-        <v>500</v>
-      </c>
-      <c r="G7" s="1">
-        <f>F7/POWER(1+F$2,E7)</f>
-        <v>396.9161205100848</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B8" s="5">
-        <v>-1000</v>
-      </c>
-      <c r="C8" s="1">
-        <f>B8/POWER(1+B$2,A8)</f>
-        <v>-822.70247479188197</v>
-      </c>
-      <c r="E8" s="9">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1500</v>
-      </c>
-      <c r="G8" s="1">
-        <f>F8/POWER(1+F$2,E8)</f>
-        <v>1102.5447791946799</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="9">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="F9" s="5">
-        <v>600</v>
-      </c>
-      <c r="G9" s="1">
-        <f>F9/POWER(1+F$2,E9)</f>
-        <v>408.34991822025182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="12">
-        <f>SUM(C5:C8)</f>
-        <v>71.801358487461471</v>
-      </c>
-      <c r="E10" s="9">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F10" s="5">
-        <f>SUM(F5:F9)*-1</f>
-        <v>-3100</v>
-      </c>
-      <c r="G10" s="1">
-        <f>F10/POWER(1+F$2,E10)</f>
-        <v>-1953.5258433376241</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="12">
-        <f>SUM(G5:G10)</f>
-        <v>396.67180586311247</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
+  <mergeCells count="8">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="A26:H26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Equities: Volatility Methods & Related Tests
PC++FP Ch2, Equities.
</commit_message>
<xml_diff>
--- a/Workbooks/Calc_Workspace.xlsx
+++ b/Workbooks/Calc_Workspace.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25035" windowHeight="11715"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25035" windowHeight="11715" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IR, CF, BM" sheetId="1" r:id="rId1"/>
+    <sheet name="Volatility" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>face</t>
   </si>
@@ -96,18 +97,45 @@
   </si>
   <si>
     <t>Bond Modeling</t>
+  </si>
+  <si>
+    <t>range vol:</t>
+  </si>
+  <si>
+    <t>std vol:</t>
+  </si>
+  <si>
+    <t>avg daily vol:</t>
+  </si>
+  <si>
+    <t>SPX Price</t>
+  </si>
+  <si>
+    <t>Book Price</t>
+  </si>
+  <si>
+    <t>Prev</t>
+  </si>
+  <si>
+    <t>Debug Info</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="9">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.0000_);[Red]\(&quot;$&quot;#,##0.0000\)"/>
-    <numFmt numFmtId="167" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="171" formatCode="#,##0.0"/>
+    <numFmt numFmtId="178" formatCode="0.000"/>
+    <numFmt numFmtId="182" formatCode="#,##0.00000000000"/>
+    <numFmt numFmtId="195" formatCode="#,##0.000000000000000000000000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +197,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,8 +236,23 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -255,8 +319,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -266,8 +356,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
@@ -283,13 +376,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="4"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -308,20 +395,48 @@
     <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8"/>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="11" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="11" applyFont="1"/>
+    <xf numFmtId="171" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="11" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="6" borderId="7" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="10"/>
+    <xf numFmtId="168" fontId="9" fillId="4" borderId="0" xfId="9" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="10" fillId="5" borderId="0" xfId="10" applyNumberFormat="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="12">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Explanatory Text" xfId="6" builtinId="53"/>
+    <cellStyle name="Good" xfId="9" builtinId="26"/>
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Heading 4" xfId="8" builtinId="19"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="10" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="11" builtinId="10"/>
     <cellStyle name="Output" xfId="3" builtinId="21"/>
     <cellStyle name="Total" xfId="7" builtinId="25"/>
     <cellStyle name="Warning Text" xfId="5" builtinId="11"/>
@@ -638,7 +753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
@@ -654,14 +769,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -709,27 +824,27 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="E11" s="13" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="E11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -895,49 +1010,49 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="15"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="11"/>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="15"/>
-      <c r="G27" s="15" t="s">
+      <c r="E27" s="23"/>
+      <c r="G27" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="H27" s="15"/>
+      <c r="H27" s="23"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="14" t="s">
         <v>19</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="16" t="s">
+      <c r="H28" s="14" t="s">
         <v>21</v>
       </c>
     </row>
@@ -945,19 +1060,19 @@
       <c r="A29" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="15">
         <v>100000</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="17">
+      <c r="E29" s="15">
         <v>200000</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="17">
+      <c r="H29" s="15">
         <v>190000</v>
       </c>
     </row>
@@ -965,19 +1080,19 @@
       <c r="A30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B30" s="15">
         <v>5000</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="15">
         <v>7500</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="17">
+      <c r="H30" s="15">
         <v>6589</v>
       </c>
     </row>
@@ -985,41 +1100,41 @@
       <c r="A31" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="18">
+      <c r="B31" s="16">
         <v>30</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="18">
+      <c r="E31" s="16">
         <v>20</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="18">
+      <c r="H31" s="16">
         <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="19">
+      <c r="B32" s="17">
         <f>B30/B29</f>
         <v>0.05</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="19">
         <f>E30/E29</f>
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H32" s="22">
+      <c r="H32" s="20">
         <f>H30/H29</f>
         <v>3.4678947368421052E-2</v>
       </c>
@@ -1028,21 +1143,21 @@
       <c r="A33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="20">
+      <c r="B33" s="18">
         <f>B29+B30*B31</f>
         <v>250000</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="20">
+      <c r="E33" s="18">
         <f>E29+E30*E31</f>
         <v>350000</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H33" s="20">
+      <c r="H33" s="18">
         <f>H29+H30*H31</f>
         <v>354725</v>
       </c>
@@ -1061,4 +1176,1300 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="W29" sqref="W29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="27">
+        <v>2381.73</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="28">
+        <f>A2-G$2</f>
+        <v>6.3134482758619015</v>
+      </c>
+      <c r="D2" s="28">
+        <f>C2*C2</f>
+        <v>39.859629131983617</v>
+      </c>
+      <c r="G2" s="25">
+        <f>AVERAGE(A2:A30)</f>
+        <v>2375.4165517241381</v>
+      </c>
+      <c r="H2">
+        <v>2375.4165517241299</v>
+      </c>
+      <c r="I2" s="4">
+        <v>3</v>
+      </c>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31">
+        <f>I2-R$3</f>
+        <v>-1.9680000000000009</v>
+      </c>
+      <c r="L2" s="31">
+        <f>K2*K2</f>
+        <v>3.8730240000000036</v>
+      </c>
+      <c r="M2" t="str">
+        <f>I2&amp;","</f>
+        <v>3,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="27">
+        <v>2365.7199999999998</v>
+      </c>
+      <c r="B3" s="31">
+        <f>ABS(A3-A2)</f>
+        <v>16.010000000000218</v>
+      </c>
+      <c r="C3" s="28">
+        <f t="shared" ref="C3:C30" si="0">A3-G$2</f>
+        <v>-9.6965517241383168</v>
+      </c>
+      <c r="D3" s="28">
+        <f t="shared" ref="D3:D30" si="1">C3*C3</f>
+        <v>94.023115338889767</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="29">
+        <f>MAX(A:A)-MIN(A:A)</f>
+        <v>73.370000000000346</v>
+      </c>
+      <c r="G3">
+        <f>SQRT(D31/(COUNT(A2:A30)-1))</f>
+        <v>22.484574279756167</v>
+      </c>
+      <c r="I3" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="J3" s="31">
+        <f>ABS(I3-I2)</f>
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="31">
+        <f t="shared" ref="K3:K11" si="2">I3-R$3</f>
+        <v>-1.4680000000000009</v>
+      </c>
+      <c r="L3" s="31">
+        <f t="shared" ref="L3:L11" si="3">K3*K3</f>
+        <v>2.1550240000000027</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M11" si="4">I3&amp;","</f>
+        <v>3.5,</v>
+      </c>
+      <c r="R3" s="37">
+        <f>AVERAGE(I2:I11)</f>
+        <v>4.9680000000000009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="27">
+        <v>2357.0300000000002</v>
+      </c>
+      <c r="B4" s="31">
+        <f t="shared" ref="B4:B30" si="5">ABS(A4-A3)</f>
+        <v>8.6899999999995998</v>
+      </c>
+      <c r="C4" s="28">
+        <f t="shared" si="0"/>
+        <v>-18.386551724137917</v>
+      </c>
+      <c r="D4" s="28">
+        <f t="shared" si="1"/>
+        <v>338.06528430439897</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="29">
+        <f>SUM(B:B)/(COUNT(B:B))</f>
+        <v>8.8382142857143435</v>
+      </c>
+      <c r="H4" s="25">
+        <f>G2-H2</f>
+        <v>8.1854523159563541E-12</v>
+      </c>
+      <c r="I4" s="4">
+        <v>5</v>
+      </c>
+      <c r="J4" s="31">
+        <f t="shared" ref="J4:J11" si="6">ABS(I4-I3)</f>
+        <v>1.5</v>
+      </c>
+      <c r="K4" s="31">
+        <f t="shared" si="2"/>
+        <v>3.199999999999914E-2</v>
+      </c>
+      <c r="L4" s="31">
+        <f t="shared" si="3"/>
+        <v>1.0239999999999449E-3</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="4"/>
+        <v>5,</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="32">
+        <f>MAX(I:I)-MIN(I:I)</f>
+        <v>3.0999999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="27">
+        <v>2400.67</v>
+      </c>
+      <c r="B5" s="31">
+        <f t="shared" si="5"/>
+        <v>43.639999999999873</v>
+      </c>
+      <c r="C5" s="28">
+        <f t="shared" si="0"/>
+        <v>25.253448275861956</v>
+      </c>
+      <c r="D5" s="28">
+        <f t="shared" si="1"/>
+        <v>637.73664982163518</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="7">
+        <f>STDEV(A:A)</f>
+        <v>22.484574279756167</v>
+      </c>
+      <c r="I5" s="4">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="J5" s="31">
+        <f t="shared" si="6"/>
+        <v>0.51999999999999957</v>
+      </c>
+      <c r="K5" s="31">
+        <f t="shared" si="2"/>
+        <v>-0.48800000000000043</v>
+      </c>
+      <c r="L5" s="31">
+        <f t="shared" si="3"/>
+        <v>0.23814400000000041</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="4"/>
+        <v>4.48,</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="32">
+        <f>SUM(J:J)/(COUNT(J:J))</f>
+        <v>0.61555555555555541</v>
+      </c>
+      <c r="R5" s="35">
+        <f>SQRT(L12/(COUNT(I2:I11)-1))</f>
+        <v>1.0295716477146104</v>
+      </c>
+      <c r="S5" s="36">
+        <f>R5-P6</f>
+        <v>5.3290705182007514E-15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="27">
+        <v>2402.3200000000002</v>
+      </c>
+      <c r="B6" s="31">
+        <f t="shared" si="5"/>
+        <v>1.6500000000000909</v>
+      </c>
+      <c r="C6" s="28">
+        <f t="shared" si="0"/>
+        <v>26.903448275862047</v>
+      </c>
+      <c r="D6" s="28">
+        <f t="shared" si="1"/>
+        <v>723.79552913198449</v>
+      </c>
+      <c r="I6" s="4">
+        <v>5.2</v>
+      </c>
+      <c r="J6" s="31">
+        <f t="shared" si="6"/>
+        <v>0.71999999999999975</v>
+      </c>
+      <c r="K6" s="31">
+        <f t="shared" si="2"/>
+        <v>0.23199999999999932</v>
+      </c>
+      <c r="L6" s="31">
+        <f t="shared" si="3"/>
+        <v>5.3823999999999685E-2</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="4"/>
+        <v>5.2,</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" s="30">
+        <f>STDEV(I:I)</f>
+        <v>1.0295716477146051</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="27">
+        <v>2390.9</v>
+      </c>
+      <c r="B7" s="31">
+        <f t="shared" si="5"/>
+        <v>11.420000000000073</v>
+      </c>
+      <c r="C7" s="28">
+        <f t="shared" si="0"/>
+        <v>15.483448275861974</v>
+      </c>
+      <c r="D7" s="28">
+        <f t="shared" si="1"/>
+        <v>239.73717051129313</v>
+      </c>
+      <c r="I7" s="4">
+        <v>6</v>
+      </c>
+      <c r="J7" s="31">
+        <f t="shared" si="6"/>
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="K7" s="31">
+        <f t="shared" si="2"/>
+        <v>1.0319999999999991</v>
+      </c>
+      <c r="L7" s="31">
+        <f t="shared" si="3"/>
+        <v>1.0650239999999982</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="4"/>
+        <v>6,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="27">
+        <v>2394.44</v>
+      </c>
+      <c r="B8" s="31">
+        <f t="shared" si="5"/>
+        <v>3.5399999999999636</v>
+      </c>
+      <c r="C8" s="28">
+        <f t="shared" si="0"/>
+        <v>19.023448275861938</v>
+      </c>
+      <c r="D8" s="28">
+        <f t="shared" si="1"/>
+        <v>361.89158430439454</v>
+      </c>
+      <c r="I8" s="4">
+        <v>6.1</v>
+      </c>
+      <c r="J8" s="31">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999645E-2</v>
+      </c>
+      <c r="K8" s="31">
+        <f t="shared" si="2"/>
+        <v>1.1319999999999988</v>
+      </c>
+      <c r="L8" s="31">
+        <f t="shared" si="3"/>
+        <v>1.2814239999999972</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="4"/>
+        <v>6.1,</v>
+      </c>
+      <c r="R8" s="35">
+        <f>SUM(I2:I11)/(COUNT(I2:I11))</f>
+        <v>4.9680000000000009</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="27">
+        <v>2399.63</v>
+      </c>
+      <c r="B9" s="31">
+        <f t="shared" si="5"/>
+        <v>5.1900000000000546</v>
+      </c>
+      <c r="C9" s="28">
+        <f t="shared" si="0"/>
+        <v>24.213448275861992</v>
+      </c>
+      <c r="D9" s="28">
+        <f t="shared" si="1"/>
+        <v>586.29107740784411</v>
+      </c>
+      <c r="I9" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="J9" s="31">
+        <f t="shared" si="6"/>
+        <v>0.59999999999999964</v>
+      </c>
+      <c r="K9" s="31">
+        <f t="shared" si="2"/>
+        <v>0.53199999999999914</v>
+      </c>
+      <c r="L9" s="31">
+        <f t="shared" si="3"/>
+        <v>0.28302399999999911</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="4"/>
+        <v>5.5,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="27">
+        <v>2396.92</v>
+      </c>
+      <c r="B10" s="31">
+        <f t="shared" si="5"/>
+        <v>2.7100000000000364</v>
+      </c>
+      <c r="C10" s="28">
+        <f t="shared" si="0"/>
+        <v>21.503448275861956</v>
+      </c>
+      <c r="D10" s="28">
+        <f t="shared" si="1"/>
+        <v>462.39828775267051</v>
+      </c>
+      <c r="I10" s="4">
+        <v>5.2</v>
+      </c>
+      <c r="J10" s="31">
+        <f t="shared" si="6"/>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="K10" s="31">
+        <f t="shared" si="2"/>
+        <v>0.23199999999999932</v>
+      </c>
+      <c r="L10" s="31">
+        <f t="shared" si="3"/>
+        <v>5.3823999999999685E-2</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="4"/>
+        <v>5.2,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="27">
+        <v>2399.38</v>
+      </c>
+      <c r="B11" s="31">
+        <f t="shared" si="5"/>
+        <v>2.4600000000000364</v>
+      </c>
+      <c r="C11" s="28">
+        <f t="shared" si="0"/>
+        <v>23.963448275861992</v>
+      </c>
+      <c r="D11" s="28">
+        <f t="shared" si="1"/>
+        <v>574.24685326991312</v>
+      </c>
+      <c r="I11" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="J11" s="31">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="31">
+        <f t="shared" si="2"/>
+        <v>0.73199999999999932</v>
+      </c>
+      <c r="L11" s="31">
+        <f t="shared" si="3"/>
+        <v>0.53582399999999897</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="4"/>
+        <v>5.7,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="27">
+        <v>2399.29</v>
+      </c>
+      <c r="B12" s="31">
+        <f t="shared" si="5"/>
+        <v>9.0000000000145519E-2</v>
+      </c>
+      <c r="C12" s="28">
+        <f t="shared" si="0"/>
+        <v>23.873448275861847</v>
+      </c>
+      <c r="D12" s="28">
+        <f t="shared" si="1"/>
+        <v>569.94153258025096</v>
+      </c>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33">
+        <f>SUBTOTAL(9,L2:L11)</f>
+        <v>9.5401600000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="27">
+        <v>2389.52</v>
+      </c>
+      <c r="B13" s="31">
+        <f t="shared" si="5"/>
+        <v>9.7699999999999818</v>
+      </c>
+      <c r="C13" s="28">
+        <f t="shared" si="0"/>
+        <v>14.103448275861865</v>
+      </c>
+      <c r="D13" s="28">
+        <f t="shared" si="1"/>
+        <v>198.90725326991102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="27">
+        <v>2388.13</v>
+      </c>
+      <c r="B14" s="31">
+        <f t="shared" si="5"/>
+        <v>1.3899999999998727</v>
+      </c>
+      <c r="C14" s="28">
+        <f t="shared" si="0"/>
+        <v>12.713448275861992</v>
+      </c>
+      <c r="D14" s="28">
+        <f t="shared" si="1"/>
+        <v>161.63176706301826</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="27">
+        <v>2391.17</v>
+      </c>
+      <c r="B15" s="31">
+        <f t="shared" si="5"/>
+        <v>3.0399999999999636</v>
+      </c>
+      <c r="C15" s="28">
+        <f t="shared" si="0"/>
+        <v>15.753448275861956</v>
+      </c>
+      <c r="D15" s="28">
+        <f t="shared" si="1"/>
+        <v>248.17113258025805</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="27">
+        <v>2388.33</v>
+      </c>
+      <c r="B16" s="31">
+        <f t="shared" si="5"/>
+        <v>2.8400000000001455</v>
+      </c>
+      <c r="C16" s="28">
+        <f t="shared" si="0"/>
+        <v>12.913448275861811</v>
+      </c>
+      <c r="D16" s="28">
+        <f t="shared" si="1"/>
+        <v>166.75714637335838</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="27">
+        <v>2384.1999999999998</v>
+      </c>
+      <c r="B17" s="31">
+        <f t="shared" si="5"/>
+        <v>4.1300000000001091</v>
+      </c>
+      <c r="C17" s="28">
+        <f t="shared" si="0"/>
+        <v>8.7834482758617014</v>
+      </c>
+      <c r="D17" s="28">
+        <f t="shared" si="1"/>
+        <v>77.148963614737895</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="27">
+        <v>2388.77</v>
+      </c>
+      <c r="B18" s="31">
+        <f t="shared" si="5"/>
+        <v>4.5700000000001637</v>
+      </c>
+      <c r="C18" s="28">
+        <f t="shared" si="0"/>
+        <v>13.353448275861865</v>
+      </c>
+      <c r="D18" s="28">
+        <f t="shared" si="1"/>
+        <v>178.31458085611823</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="27">
+        <v>2387.4499999999998</v>
+      </c>
+      <c r="B19" s="31">
+        <f t="shared" si="5"/>
+        <v>1.3200000000001637</v>
+      </c>
+      <c r="C19" s="28">
+        <f t="shared" si="0"/>
+        <v>12.033448275861701</v>
+      </c>
+      <c r="D19" s="28">
+        <f t="shared" si="1"/>
+        <v>144.80387740783897</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="27">
+        <v>2388.61</v>
+      </c>
+      <c r="B20" s="31">
+        <f t="shared" si="5"/>
+        <v>1.1600000000003092</v>
+      </c>
+      <c r="C20" s="28">
+        <f t="shared" si="0"/>
+        <v>13.193448275862011</v>
+      </c>
+      <c r="D20" s="28">
+        <f t="shared" si="1"/>
+        <v>174.06707740784626</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="27">
+        <v>2374.15</v>
+      </c>
+      <c r="B21" s="31">
+        <f t="shared" si="5"/>
+        <v>14.460000000000036</v>
+      </c>
+      <c r="C21" s="28">
+        <f t="shared" si="0"/>
+        <v>-1.2665517241380257</v>
+      </c>
+      <c r="D21" s="28">
+        <f t="shared" si="1"/>
+        <v>1.6041532699170056</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="27">
+        <v>2348.69</v>
+      </c>
+      <c r="B22" s="31">
+        <f t="shared" si="5"/>
+        <v>25.460000000000036</v>
+      </c>
+      <c r="C22" s="28">
+        <f t="shared" si="0"/>
+        <v>-26.726551724138062</v>
+      </c>
+      <c r="D22" s="28">
+        <f t="shared" si="1"/>
+        <v>714.30856706302723</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="27">
+        <v>2355.84</v>
+      </c>
+      <c r="B23" s="31">
+        <f t="shared" si="5"/>
+        <v>7.1500000000000909</v>
+      </c>
+      <c r="C23" s="28">
+        <f t="shared" si="0"/>
+        <v>-19.576551724137971</v>
+      </c>
+      <c r="D23" s="28">
+        <f t="shared" si="1"/>
+        <v>383.24137740784937</v>
+      </c>
+      <c r="K23" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="40"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="40"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="27">
+        <v>2338.17</v>
+      </c>
+      <c r="B24" s="31">
+        <f t="shared" si="5"/>
+        <v>17.670000000000073</v>
+      </c>
+      <c r="C24" s="28">
+        <f t="shared" si="0"/>
+        <v>-37.246551724138044</v>
+      </c>
+      <c r="D24" s="28">
+        <f t="shared" si="1"/>
+        <v>1387.3056153388907</v>
+      </c>
+      <c r="K24">
+        <v>2381.73</v>
+      </c>
+      <c r="L24" s="24"/>
+      <c r="O24">
+        <v>39.859629131983617</v>
+      </c>
+      <c r="Q24">
+        <v>39.859629131983603</v>
+      </c>
+      <c r="R24" s="39">
+        <f>O24-Q24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="27">
+        <v>2342.19</v>
+      </c>
+      <c r="B25" s="31">
+        <f t="shared" si="5"/>
+        <v>4.0199999999999818</v>
+      </c>
+      <c r="C25" s="28">
+        <f t="shared" si="0"/>
+        <v>-33.226551724138062</v>
+      </c>
+      <c r="D25" s="28">
+        <f t="shared" si="1"/>
+        <v>1104.0037394768219</v>
+      </c>
+      <c r="K25">
+        <v>2365.7199999999998</v>
+      </c>
+      <c r="L25" s="24"/>
+      <c r="O25">
+        <v>94.023115338889767</v>
+      </c>
+      <c r="Q25">
+        <v>94.023115338889696</v>
+      </c>
+      <c r="R25" s="39">
+        <f t="shared" ref="R25:R52" si="7">O25-Q25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="27">
+        <v>2349.0100000000002</v>
+      </c>
+      <c r="B26" s="31">
+        <f t="shared" si="5"/>
+        <v>6.8200000000001637</v>
+      </c>
+      <c r="C26" s="28">
+        <f t="shared" si="0"/>
+        <v>-26.406551724137898</v>
+      </c>
+      <c r="D26" s="28">
+        <f t="shared" si="1"/>
+        <v>697.30597395957022</v>
+      </c>
+      <c r="K26">
+        <v>2357.0300000000002</v>
+      </c>
+      <c r="L26" s="24"/>
+      <c r="O26">
+        <v>338.06528430439897</v>
+      </c>
+      <c r="Q26">
+        <v>338.06528430439801</v>
+      </c>
+      <c r="R26" s="39">
+        <f t="shared" si="7"/>
+        <v>9.6633812063373625E-13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="27">
+        <v>2328.9499999999998</v>
+      </c>
+      <c r="B27" s="31">
+        <f t="shared" si="5"/>
+        <v>20.0600000000004</v>
+      </c>
+      <c r="C27" s="28">
+        <f t="shared" si="0"/>
+        <v>-46.466551724138299</v>
+      </c>
+      <c r="D27" s="28">
+        <f t="shared" si="1"/>
+        <v>2159.14042913202</v>
+      </c>
+      <c r="K27">
+        <v>2400.67</v>
+      </c>
+      <c r="L27" s="24"/>
+      <c r="O27">
+        <v>637.73664982163518</v>
+      </c>
+      <c r="Q27">
+        <v>637.73664982163496</v>
+      </c>
+      <c r="R27" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="27">
+        <v>2344.9299999999998</v>
+      </c>
+      <c r="B28" s="31">
+        <f t="shared" si="5"/>
+        <v>15.980000000000018</v>
+      </c>
+      <c r="C28" s="28">
+        <f t="shared" si="0"/>
+        <v>-30.48655172413828</v>
+      </c>
+      <c r="D28" s="28">
+        <f t="shared" si="1"/>
+        <v>929.42983602855873</v>
+      </c>
+      <c r="E28" s="24"/>
+      <c r="F28">
+        <v>13611</v>
+      </c>
+      <c r="K28">
+        <v>2402.3200000000002</v>
+      </c>
+      <c r="L28" s="24"/>
+      <c r="O28">
+        <v>723.79552913198449</v>
+      </c>
+      <c r="Q28">
+        <v>723.79552913198404</v>
+      </c>
+      <c r="R28" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="27">
+        <v>2353.7800000000002</v>
+      </c>
+      <c r="B29" s="31">
+        <f t="shared" si="5"/>
+        <v>8.8500000000003638</v>
+      </c>
+      <c r="C29" s="28">
+        <f t="shared" si="0"/>
+        <v>-21.636551724137917</v>
+      </c>
+      <c r="D29" s="28">
+        <f t="shared" si="1"/>
+        <v>468.14037051129543</v>
+      </c>
+      <c r="K29">
+        <v>2390.9</v>
+      </c>
+      <c r="L29" s="24"/>
+      <c r="O29">
+        <v>239.73717051129313</v>
+      </c>
+      <c r="Q29">
+        <v>239.73717051129299</v>
+      </c>
+      <c r="R29" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="27">
+        <v>2357.16</v>
+      </c>
+      <c r="B30" s="31">
+        <f t="shared" si="5"/>
+        <v>3.3799999999996544</v>
+      </c>
+      <c r="C30" s="28">
+        <f t="shared" si="0"/>
+        <v>-18.256551724138262</v>
+      </c>
+      <c r="D30" s="28">
+        <f t="shared" si="1"/>
+        <v>333.30168085613576</v>
+      </c>
+      <c r="K30">
+        <v>2394.44</v>
+      </c>
+      <c r="L30" s="24"/>
+      <c r="O30">
+        <v>361.89158430439454</v>
+      </c>
+      <c r="Q30">
+        <v>361.89158430439397</v>
+      </c>
+      <c r="R30" s="39">
+        <f t="shared" si="7"/>
+        <v>5.6843418860808015E-13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D31" s="34">
+        <f>SUBTOTAL(9,D2:D30)</f>
+        <v>14155.570255172432</v>
+      </c>
+      <c r="K31">
+        <v>2399.63</v>
+      </c>
+      <c r="L31" s="24"/>
+      <c r="O31">
+        <v>586.29107740784411</v>
+      </c>
+      <c r="Q31">
+        <v>586.291077407844</v>
+      </c>
+      <c r="R31" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <v>2396.92</v>
+      </c>
+      <c r="L32" s="24"/>
+      <c r="O32">
+        <v>462.39828775267051</v>
+      </c>
+      <c r="Q32">
+        <v>462.39828775267</v>
+      </c>
+      <c r="R32" s="39">
+        <f t="shared" si="7"/>
+        <v>5.1159076974727213E-13</v>
+      </c>
+    </row>
+    <row r="33" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D33" s="24">
+        <f>SUM(D2:D30)</f>
+        <v>14155.570255172432</v>
+      </c>
+      <c r="K33">
+        <v>2399.38</v>
+      </c>
+      <c r="L33" s="24"/>
+      <c r="O33">
+        <v>574.24685326991312</v>
+      </c>
+      <c r="Q33">
+        <v>574.246853269913</v>
+      </c>
+      <c r="R33" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>14155.570255172401</v>
+      </c>
+      <c r="K34">
+        <v>2399.29</v>
+      </c>
+      <c r="L34" s="24"/>
+      <c r="O34">
+        <v>569.94153258025096</v>
+      </c>
+      <c r="Q34">
+        <v>569.94153258025005</v>
+      </c>
+      <c r="R34" s="39">
+        <f t="shared" si="7"/>
+        <v>9.0949470177292824E-13</v>
+      </c>
+    </row>
+    <row r="35" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D35" s="38">
+        <f>D34-D33</f>
+        <v>-3.092281986027956E-11</v>
+      </c>
+      <c r="K35">
+        <v>2389.52</v>
+      </c>
+      <c r="L35" s="24"/>
+      <c r="O35">
+        <v>198.90725326991102</v>
+      </c>
+      <c r="Q35">
+        <v>198.907253269911</v>
+      </c>
+      <c r="R35" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K36">
+        <v>2388.13</v>
+      </c>
+      <c r="L36" s="24"/>
+      <c r="O36">
+        <v>161.63176706301826</v>
+      </c>
+      <c r="Q36">
+        <v>161.631767063018</v>
+      </c>
+      <c r="R36" s="39">
+        <f t="shared" si="7"/>
+        <v>2.5579538487363607E-13</v>
+      </c>
+    </row>
+    <row r="37" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <v>2391.17</v>
+      </c>
+      <c r="L37" s="24"/>
+      <c r="O37">
+        <v>248.17113258025805</v>
+      </c>
+      <c r="Q37">
+        <v>248.17113258025799</v>
+      </c>
+      <c r="R37" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <v>2388.33</v>
+      </c>
+      <c r="L38" s="24"/>
+      <c r="O38">
+        <v>166.75714637335838</v>
+      </c>
+      <c r="Q38">
+        <v>166.75714637335801</v>
+      </c>
+      <c r="R38" s="39">
+        <f t="shared" si="7"/>
+        <v>3.694822225952521E-13</v>
+      </c>
+    </row>
+    <row r="39" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K39">
+        <v>2384.1999999999998</v>
+      </c>
+      <c r="L39" s="24"/>
+      <c r="O39">
+        <v>77.148963614737895</v>
+      </c>
+      <c r="Q39">
+        <v>77.148963614737795</v>
+      </c>
+      <c r="R39" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K40">
+        <v>2388.77</v>
+      </c>
+      <c r="L40" s="24"/>
+      <c r="O40">
+        <v>178.31458085611823</v>
+      </c>
+      <c r="Q40">
+        <v>178.314580856118</v>
+      </c>
+      <c r="R40" s="39">
+        <f t="shared" si="7"/>
+        <v>2.2737367544323206E-13</v>
+      </c>
+    </row>
+    <row r="41" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K41">
+        <v>2387.4499999999998</v>
+      </c>
+      <c r="L41" s="24"/>
+      <c r="O41">
+        <v>144.80387740783897</v>
+      </c>
+      <c r="Q41">
+        <v>144.803877407838</v>
+      </c>
+      <c r="R41" s="39">
+        <f t="shared" si="7"/>
+        <v>9.6633812063373625E-13</v>
+      </c>
+    </row>
+    <row r="42" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K42">
+        <v>2388.61</v>
+      </c>
+      <c r="L42" s="24"/>
+      <c r="O42">
+        <v>174.06707740784626</v>
+      </c>
+      <c r="Q42">
+        <v>174.067077407846</v>
+      </c>
+      <c r="R42" s="39">
+        <f t="shared" si="7"/>
+        <v>2.5579538487363607E-13</v>
+      </c>
+    </row>
+    <row r="43" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K43">
+        <v>2374.15</v>
+      </c>
+      <c r="L43" s="24"/>
+      <c r="O43">
+        <v>1.6041532699170056</v>
+      </c>
+      <c r="Q43">
+        <v>1.604153269917</v>
+      </c>
+      <c r="R43" s="39">
+        <f t="shared" si="7"/>
+        <v>5.5511151231257827E-15</v>
+      </c>
+    </row>
+    <row r="44" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K44">
+        <v>2348.69</v>
+      </c>
+      <c r="L44" s="24"/>
+      <c r="O44">
+        <v>714.30856706302723</v>
+      </c>
+      <c r="Q44">
+        <v>714.308567063027</v>
+      </c>
+      <c r="R44" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K45">
+        <v>2355.84</v>
+      </c>
+      <c r="L45" s="24"/>
+      <c r="O45">
+        <v>383.24137740784937</v>
+      </c>
+      <c r="Q45">
+        <v>383.24137740784897</v>
+      </c>
+      <c r="R45" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K46">
+        <v>2338.17</v>
+      </c>
+      <c r="L46" s="24"/>
+      <c r="O46">
+        <v>1387.3056153388907</v>
+      </c>
+      <c r="Q46">
+        <v>1387.30561533889</v>
+      </c>
+      <c r="R46" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K47">
+        <v>2342.19</v>
+      </c>
+      <c r="L47" s="24"/>
+      <c r="O47">
+        <v>1104.0037394768219</v>
+      </c>
+      <c r="Q47">
+        <v>1104.0037394768201</v>
+      </c>
+      <c r="R47" s="39">
+        <f t="shared" si="7"/>
+        <v>1.8189894035458565E-12</v>
+      </c>
+    </row>
+    <row r="48" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K48">
+        <v>2349.0100000000002</v>
+      </c>
+      <c r="L48" s="24"/>
+      <c r="O48">
+        <v>697.30597395957022</v>
+      </c>
+      <c r="Q48">
+        <v>697.30597395957</v>
+      </c>
+      <c r="R48" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K49">
+        <v>2328.9499999999998</v>
+      </c>
+      <c r="L49" s="24"/>
+      <c r="O49">
+        <v>2159.14042913202</v>
+      </c>
+      <c r="Q49">
+        <v>2159.14042913202</v>
+      </c>
+      <c r="R49" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K50">
+        <v>2344.9299999999998</v>
+      </c>
+      <c r="L50" s="24"/>
+      <c r="O50">
+        <v>929.42983602855873</v>
+      </c>
+      <c r="Q50">
+        <v>929.42983602855804</v>
+      </c>
+      <c r="R50" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K51">
+        <v>2353.7800000000002</v>
+      </c>
+      <c r="L51" s="24"/>
+      <c r="O51">
+        <v>468.14037051129543</v>
+      </c>
+      <c r="Q51">
+        <v>468.14037051129498</v>
+      </c>
+      <c r="R51" s="39">
+        <f t="shared" si="7"/>
+        <v>4.5474735088646412E-13</v>
+      </c>
+    </row>
+    <row r="52" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K52">
+        <v>2357.16</v>
+      </c>
+      <c r="L52" s="24"/>
+      <c r="O52">
+        <v>333.30168085613576</v>
+      </c>
+      <c r="Q52">
+        <v>333.30168085613502</v>
+      </c>
+      <c r="R52" s="39">
+        <f t="shared" si="7"/>
+        <v>7.3896444519050419E-13</v>
+      </c>
+    </row>
+    <row r="53" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="O53">
+        <f>SUBTOTAL(9,O24:O52)</f>
+        <v>14155.570255172432</v>
+      </c>
+      <c r="Q53">
+        <f>SUBTOTAL(9,Q24:Q52)</f>
+        <v>14155.570255172421</v>
+      </c>
+      <c r="T53">
+        <f>SQRT(Q53/(COUNT(Q24:Q52)-1))</f>
+        <v>22.48457427975616</v>
+      </c>
+    </row>
+    <row r="55" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="P55">
+        <f>O53-Q53</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K23:R23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a basic fundamentals calculator  w/ definitions in the spreadsheet. Basic test case setup and clean.
</commit_message>
<xml_diff>
--- a/Workbooks/Calc_Workspace.xlsx
+++ b/Workbooks/Calc_Workspace.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25035" windowHeight="11715" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25035" windowHeight="11715" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="IR, CF, BM" sheetId="1" r:id="rId1"/>
     <sheet name="Volatility" sheetId="2" r:id="rId2"/>
     <sheet name="Correlation" sheetId="4" r:id="rId3"/>
+    <sheet name="Fundamentals" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="BSE_Close">Correlation!$F$2:$F$31</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="116">
   <si>
     <t>face</t>
   </si>
@@ -281,6 +282,108 @@
   </si>
   <si>
     <t>Book Examples</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Calc</t>
+  </si>
+  <si>
+    <t>Price-earnings ratio</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>P/E</t>
+  </si>
+  <si>
+    <t>Calculated as the price of the total stock of the company (price * shares outstanding), divided by the earnings as published in the last quarter release.</t>
+  </si>
+  <si>
+    <t>Book Value</t>
+  </si>
+  <si>
+    <t>BV</t>
+  </si>
+  <si>
+    <t>The book value corresponds to the amount of assets currently on the company balance sheet. This is in essence an accounting measure of the value of the company, without considering market factors such as future earnings, for example.</t>
+  </si>
+  <si>
+    <t>Price-to-book ratio</t>
+  </si>
+  <si>
+    <t>B/P</t>
+  </si>
+  <si>
+    <t>This ratio is determined by dividing the stock price by the assets minus liabilities.</t>
+  </si>
+  <si>
+    <t>Stock Price / Assets - Liabilities and IntangiableAssets</t>
+  </si>
+  <si>
+    <t>(Price * Shares Outstanding) / Earnings</t>
+  </si>
+  <si>
+    <t>TotalAssets - IngangibleAssets</t>
+  </si>
+  <si>
+    <t>This only includes tangible assets</t>
+  </si>
+  <si>
+    <t>Price-earnings to growth</t>
+  </si>
+  <si>
+    <t>PEG</t>
+  </si>
+  <si>
+    <t>This indicator can be used to compare companies with similar P/E, but different growth rates.</t>
+  </si>
+  <si>
+    <t>(P/E) / EPS Annual Growth</t>
+  </si>
+  <si>
+    <t>Earnings Before Interest, taxes, depreciation, and amortization</t>
+  </si>
+  <si>
+    <t>EBITDA</t>
+  </si>
+  <si>
+    <t>This is a measure that can be used to determine how a company is making a profit, and it is based on accounting information provided by the company in every earnings release. The value simply represents how much profit the company made befre items such as taxes and related expenses were paid.</t>
+  </si>
+  <si>
+    <t>Operating Profit + Amortization Expenses + Depreciation Expenses</t>
+  </si>
+  <si>
+    <t>Return on Equity</t>
+  </si>
+  <si>
+    <t>ROE</t>
+  </si>
+  <si>
+    <t>This ratio is used to determine the percentage of net income generated based on shareholder's equity. Investors are usually interested in companies able to generate higher income on thes ame amount of equity.</t>
+  </si>
+  <si>
+    <t>NetIncome / ShareholdersEquity</t>
+  </si>
+  <si>
+    <t>Forward P/E</t>
+  </si>
+  <si>
+    <t>F/PE</t>
+  </si>
+  <si>
+    <t>This number is similar to the P/E ratio, but instead of being calculated based on existing revenue data, it is a prediction for the next quarter made by analysts. When compared to P/E, this number can be used to determien if analyst expect the revenue to increase , decrease, or say at the same levels.</t>
+  </si>
+  <si>
+    <t>(Price * Shares Outstanding) / Future Estimated Earnings</t>
   </si>
 </sst>
 </file>
@@ -602,7 +705,7 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
@@ -676,6 +779,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="10" fillId="5" borderId="0" xfId="10" applyNumberFormat="1"/>
     <xf numFmtId="173" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="174" fontId="11" fillId="7" borderId="8" xfId="12" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="12"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -691,14 +799,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="174" fontId="11" fillId="7" borderId="8" xfId="12" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="12"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -715,7 +827,29 @@
     <cellStyle name="Total" xfId="7" builtinId="25"/>
     <cellStyle name="Warning Text" xfId="5" builtinId="11"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -780,91 +914,91 @@
             <c:strLit>
               <c:ptCount val="29"/>
               <c:pt idx="0">
-                <c:v>2.00</c:v>
+                <c:v>2</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>3.00</c:v>
+                <c:v>3</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>4.00</c:v>
+                <c:v>4</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>5.00</c:v>
+                <c:v>5</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>6.00</c:v>
+                <c:v>6</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>7.00</c:v>
+                <c:v>7</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>8.00</c:v>
+                <c:v>8</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>9.00</c:v>
+                <c:v>9</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v>10.00</c:v>
+                <c:v>10</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>11.00</c:v>
+                <c:v>11</c:v>
               </c:pt>
               <c:pt idx="10">
-                <c:v>12.00</c:v>
+                <c:v>12</c:v>
               </c:pt>
               <c:pt idx="11">
-                <c:v>13.00</c:v>
+                <c:v>13</c:v>
               </c:pt>
               <c:pt idx="12">
-                <c:v>14.00</c:v>
+                <c:v>14</c:v>
               </c:pt>
               <c:pt idx="13">
-                <c:v>15.00</c:v>
+                <c:v>15</c:v>
               </c:pt>
               <c:pt idx="14">
-                <c:v>16.00</c:v>
+                <c:v>16</c:v>
               </c:pt>
               <c:pt idx="15">
-                <c:v>17.00</c:v>
+                <c:v>17</c:v>
               </c:pt>
               <c:pt idx="16">
-                <c:v>18.00</c:v>
+                <c:v>18</c:v>
               </c:pt>
               <c:pt idx="17">
-                <c:v>19.00</c:v>
+                <c:v>19</c:v>
               </c:pt>
               <c:pt idx="18">
-                <c:v>20.00</c:v>
+                <c:v>20</c:v>
               </c:pt>
               <c:pt idx="19">
-                <c:v>21.00</c:v>
+                <c:v>21</c:v>
               </c:pt>
               <c:pt idx="20">
-                <c:v>22.00</c:v>
+                <c:v>22</c:v>
               </c:pt>
               <c:pt idx="21">
-                <c:v>23.00</c:v>
+                <c:v>23</c:v>
               </c:pt>
               <c:pt idx="22">
-                <c:v>24.00</c:v>
+                <c:v>24</c:v>
               </c:pt>
               <c:pt idx="23">
-                <c:v>25.00</c:v>
+                <c:v>25</c:v>
               </c:pt>
               <c:pt idx="24">
-                <c:v>26.00</c:v>
+                <c:v>26</c:v>
               </c:pt>
               <c:pt idx="25">
-                <c:v>27.00</c:v>
+                <c:v>27</c:v>
               </c:pt>
               <c:pt idx="26">
-                <c:v>28.00</c:v>
+                <c:v>28</c:v>
               </c:pt>
               <c:pt idx="27">
-                <c:v>29.00</c:v>
+                <c:v>29</c:v>
               </c:pt>
               <c:pt idx="28">
-                <c:v>30.00</c:v>
+                <c:v>30</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -1005,91 +1139,91 @@
             <c:strLit>
               <c:ptCount val="29"/>
               <c:pt idx="0">
-                <c:v>2</c:v>
+                <c:v>2.00</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>3</c:v>
+                <c:v>3.00</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>4</c:v>
+                <c:v>4.00</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>5</c:v>
+                <c:v>5.00</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>6</c:v>
+                <c:v>6.00</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>7</c:v>
+                <c:v>7.00</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>8</c:v>
+                <c:v>8.00</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>9</c:v>
+                <c:v>9.00</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v>10</c:v>
+                <c:v>10.00</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>11</c:v>
+                <c:v>11.00</c:v>
               </c:pt>
               <c:pt idx="10">
-                <c:v>12</c:v>
+                <c:v>12.00</c:v>
               </c:pt>
               <c:pt idx="11">
-                <c:v>13</c:v>
+                <c:v>13.00</c:v>
               </c:pt>
               <c:pt idx="12">
-                <c:v>14</c:v>
+                <c:v>14.00</c:v>
               </c:pt>
               <c:pt idx="13">
-                <c:v>15</c:v>
+                <c:v>15.00</c:v>
               </c:pt>
               <c:pt idx="14">
-                <c:v>16</c:v>
+                <c:v>16.00</c:v>
               </c:pt>
               <c:pt idx="15">
-                <c:v>17</c:v>
+                <c:v>17.00</c:v>
               </c:pt>
               <c:pt idx="16">
-                <c:v>18</c:v>
+                <c:v>18.00</c:v>
               </c:pt>
               <c:pt idx="17">
-                <c:v>19</c:v>
+                <c:v>19.00</c:v>
               </c:pt>
               <c:pt idx="18">
-                <c:v>20</c:v>
+                <c:v>20.00</c:v>
               </c:pt>
               <c:pt idx="19">
-                <c:v>21</c:v>
+                <c:v>21.00</c:v>
               </c:pt>
               <c:pt idx="20">
-                <c:v>22</c:v>
+                <c:v>22.00</c:v>
               </c:pt>
               <c:pt idx="21">
-                <c:v>23</c:v>
+                <c:v>23.00</c:v>
               </c:pt>
               <c:pt idx="22">
-                <c:v>24</c:v>
+                <c:v>24.00</c:v>
               </c:pt>
               <c:pt idx="23">
-                <c:v>25</c:v>
+                <c:v>25.00</c:v>
               </c:pt>
               <c:pt idx="24">
-                <c:v>26</c:v>
+                <c:v>26.00</c:v>
               </c:pt>
               <c:pt idx="25">
-                <c:v>27</c:v>
+                <c:v>27.00</c:v>
               </c:pt>
               <c:pt idx="26">
-                <c:v>28</c:v>
+                <c:v>28.00</c:v>
               </c:pt>
               <c:pt idx="27">
-                <c:v>29</c:v>
+                <c:v>29.00</c:v>
               </c:pt>
               <c:pt idx="28">
-                <c:v>30</c:v>
+                <c:v>30.00</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -1969,6 +2103,20 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:E1048576"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Metric" dataDxfId="6"/>
+    <tableColumn id="5" name="Alias" dataDxfId="5"/>
+    <tableColumn id="2" name="Definition" dataDxfId="4"/>
+    <tableColumn id="3" name="Notes" dataDxfId="3"/>
+    <tableColumn id="4" name="Calc" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2284,14 +2432,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -2339,27 +2487,27 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="E11" s="50" t="s">
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="E11" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2525,31 +2673,31 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="51"/>
+      <c r="B27" s="54"/>
       <c r="C27" s="11"/>
-      <c r="D27" s="51" t="s">
+      <c r="D27" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="51"/>
-      <c r="G27" s="51" t="s">
+      <c r="E27" s="54"/>
+      <c r="G27" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="H27" s="51"/>
+      <c r="H27" s="54"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -3361,16 +3509,16 @@
         <f t="shared" si="1"/>
         <v>383.24137740784937</v>
       </c>
-      <c r="K23" s="52" t="s">
+      <c r="K23" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="52"/>
-      <c r="P23" s="52"/>
-      <c r="Q23" s="52"/>
-      <c r="R23" s="52"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="55"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="24">
@@ -3993,7 +4141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="X32" sqref="X32:X38"/>
     </sheetView>
   </sheetViews>
@@ -4659,12 +4807,12 @@
         <f>K14*K13</f>
         <v>2582.75086871556</v>
       </c>
-      <c r="U16" s="55" t="s">
+      <c r="U16" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="V16" s="55"/>
-      <c r="W16" s="55"/>
-      <c r="X16" s="55"/>
+      <c r="V16" s="57"/>
+      <c r="W16" s="57"/>
+      <c r="X16" s="57"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -4694,14 +4842,14 @@
         <v>13112.98,</v>
       </c>
       <c r="I17" s="21"/>
-      <c r="U17" s="53">
+      <c r="U17" s="56">
         <v>1</v>
       </c>
-      <c r="V17" s="53"/>
-      <c r="W17" s="53">
+      <c r="V17" s="56"/>
+      <c r="W17" s="56">
         <v>2</v>
       </c>
-      <c r="X17" s="53"/>
+      <c r="X17" s="56"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -4731,16 +4879,16 @@
         <v>13167.6,</v>
       </c>
       <c r="I18" s="21"/>
-      <c r="U18" s="54" t="s">
+      <c r="U18" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="V18" s="54" t="s">
+      <c r="V18" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="W18" s="54" t="s">
+      <c r="W18" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="X18" s="54" t="s">
+      <c r="X18" s="49" t="s">
         <v>75</v>
       </c>
     </row>
@@ -5101,7 +5249,7 @@
       <c r="V26">
         <v>3.1</v>
       </c>
-      <c r="W26" s="57">
+      <c r="W26" s="51">
         <f>CORREL(W19:W25,X19:X25)</f>
         <v>-1</v>
       </c>
@@ -5229,7 +5377,7 @@
         <f t="shared" si="5"/>
         <v>8.8387825463574016E-2</v>
       </c>
-      <c r="U29" s="56">
+      <c r="U29" s="50">
         <f>CORREL(U19:U28,V19:V28)</f>
         <v>-5.0600991587674081E-2</v>
       </c>
@@ -6433,4 +6581,326 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="23.7109375" style="58"/>
+    <col min="3" max="3" width="54.140625" style="58" customWidth="1"/>
+    <col min="4" max="5" width="23.7109375" style="58"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="59" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="59"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="59"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="59"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="59"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="59"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="59"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="59"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="59"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="59"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="59"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="59"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="59"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="59"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="59"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="59"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="59"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="59"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="59"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="59"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="59"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="59"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="59"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="59"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="59"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Analyst Recommendations & Recommendation Processor.
</commit_message>
<xml_diff>
--- a/Workbooks/Calc_Workspace.xlsx
+++ b/Workbooks/Calc_Workspace.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25035" windowHeight="11715" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25035" windowHeight="11715" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="IR, CF, BM" sheetId="1" r:id="rId1"/>
     <sheet name="Volatility" sheetId="2" r:id="rId2"/>
     <sheet name="Correlation" sheetId="4" r:id="rId3"/>
     <sheet name="Fundamentals" sheetId="5" r:id="rId4"/>
+    <sheet name="Debug" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="BSE_Close">Correlation!$F$2:$F$31</definedName>
@@ -784,6 +785,15 @@
     </xf>
     <xf numFmtId="174" fontId="11" fillId="7" borderId="8" xfId="12" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="12"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -801,15 +811,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -883,8 +884,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.1191832921195098E-2"/>
-          <c:y val="2.4456500172899551E-2"/>
+          <c:x val="8.846124162311135E-2"/>
+          <c:y val="4.1735117883482706E-2"/>
           <c:w val="0.89586763782044365"/>
           <c:h val="0.90420653300690357"/>
         </c:manualLayout>
@@ -914,91 +915,91 @@
             <c:strLit>
               <c:ptCount val="29"/>
               <c:pt idx="0">
-                <c:v>2</c:v>
+                <c:v>2.00</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>3</c:v>
+                <c:v>3.00</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>4</c:v>
+                <c:v>4.00</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>5</c:v>
+                <c:v>5.00</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>6</c:v>
+                <c:v>6.00</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>7</c:v>
+                <c:v>7.00</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>8</c:v>
+                <c:v>8.00</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>9</c:v>
+                <c:v>9.00</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v>10</c:v>
+                <c:v>10.00</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>11</c:v>
+                <c:v>11.00</c:v>
               </c:pt>
               <c:pt idx="10">
-                <c:v>12</c:v>
+                <c:v>12.00</c:v>
               </c:pt>
               <c:pt idx="11">
-                <c:v>13</c:v>
+                <c:v>13.00</c:v>
               </c:pt>
               <c:pt idx="12">
-                <c:v>14</c:v>
+                <c:v>14.00</c:v>
               </c:pt>
               <c:pt idx="13">
-                <c:v>15</c:v>
+                <c:v>15.00</c:v>
               </c:pt>
               <c:pt idx="14">
-                <c:v>16</c:v>
+                <c:v>16.00</c:v>
               </c:pt>
               <c:pt idx="15">
-                <c:v>17</c:v>
+                <c:v>17.00</c:v>
               </c:pt>
               <c:pt idx="16">
-                <c:v>18</c:v>
+                <c:v>18.00</c:v>
               </c:pt>
               <c:pt idx="17">
-                <c:v>19</c:v>
+                <c:v>19.00</c:v>
               </c:pt>
               <c:pt idx="18">
-                <c:v>20</c:v>
+                <c:v>20.00</c:v>
               </c:pt>
               <c:pt idx="19">
-                <c:v>21</c:v>
+                <c:v>21.00</c:v>
               </c:pt>
               <c:pt idx="20">
-                <c:v>22</c:v>
+                <c:v>22.00</c:v>
               </c:pt>
               <c:pt idx="21">
-                <c:v>23</c:v>
+                <c:v>23.00</c:v>
               </c:pt>
               <c:pt idx="22">
-                <c:v>24</c:v>
+                <c:v>24.00</c:v>
               </c:pt>
               <c:pt idx="23">
-                <c:v>25</c:v>
+                <c:v>25.00</c:v>
               </c:pt>
               <c:pt idx="24">
-                <c:v>26</c:v>
+                <c:v>26.00</c:v>
               </c:pt>
               <c:pt idx="25">
-                <c:v>27</c:v>
+                <c:v>27.00</c:v>
               </c:pt>
               <c:pt idx="26">
-                <c:v>28</c:v>
+                <c:v>28.00</c:v>
               </c:pt>
               <c:pt idx="27">
-                <c:v>29</c:v>
+                <c:v>29.00</c:v>
               </c:pt>
               <c:pt idx="28">
-                <c:v>30</c:v>
+                <c:v>30.00</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -2104,14 +2105,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E1048576"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Metric" dataDxfId="6"/>
-    <tableColumn id="5" name="Alias" dataDxfId="5"/>
-    <tableColumn id="2" name="Definition" dataDxfId="4"/>
-    <tableColumn id="3" name="Notes" dataDxfId="3"/>
-    <tableColumn id="4" name="Calc" dataDxfId="2"/>
+    <tableColumn id="1" name="Metric" dataDxfId="4"/>
+    <tableColumn id="5" name="Alias" dataDxfId="3"/>
+    <tableColumn id="2" name="Definition" dataDxfId="2"/>
+    <tableColumn id="3" name="Notes" dataDxfId="1"/>
+    <tableColumn id="4" name="Calc" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2432,14 +2433,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -2487,27 +2488,27 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="E11" s="53" t="s">
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="E11" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2673,31 +2674,31 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="54" t="s">
+      <c r="A27" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="54"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="11"/>
-      <c r="D27" s="54" t="s">
+      <c r="D27" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="54"/>
-      <c r="G27" s="54" t="s">
+      <c r="E27" s="57"/>
+      <c r="G27" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H27" s="54"/>
+      <c r="H27" s="57"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -2846,7 +2847,7 @@
   <dimension ref="A1:T55"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3509,16 +3510,16 @@
         <f t="shared" si="1"/>
         <v>383.24137740784937</v>
       </c>
-      <c r="K23" s="55" t="s">
+      <c r="K23" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="L23" s="55"/>
-      <c r="M23" s="55"/>
-      <c r="N23" s="55"/>
-      <c r="O23" s="55"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="55"/>
-      <c r="R23" s="55"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="58"/>
+      <c r="O23" s="58"/>
+      <c r="P23" s="58"/>
+      <c r="Q23" s="58"/>
+      <c r="R23" s="58"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="24">
@@ -4141,8 +4142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X63"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="X32" sqref="X32:X38"/>
+    <sheetView showGridLines="0" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4807,12 +4808,12 @@
         <f>K14*K13</f>
         <v>2582.75086871556</v>
       </c>
-      <c r="U16" s="57" t="s">
+      <c r="U16" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="V16" s="57"/>
-      <c r="W16" s="57"/>
-      <c r="X16" s="57"/>
+      <c r="V16" s="60"/>
+      <c r="W16" s="60"/>
+      <c r="X16" s="60"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -4842,14 +4843,14 @@
         <v>13112.98,</v>
       </c>
       <c r="I17" s="21"/>
-      <c r="U17" s="56">
+      <c r="U17" s="59">
         <v>1</v>
       </c>
-      <c r="V17" s="56"/>
-      <c r="W17" s="56">
+      <c r="V17" s="59"/>
+      <c r="W17" s="59">
         <v>2</v>
       </c>
-      <c r="X17" s="56"/>
+      <c r="X17" s="59"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -6587,315 +6588,315 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="23.7109375" style="58"/>
-    <col min="3" max="3" width="54.140625" style="58" customWidth="1"/>
-    <col min="4" max="5" width="23.7109375" style="58"/>
+    <col min="1" max="2" width="23.7109375" style="52"/>
+    <col min="3" max="3" width="54.140625" style="52" customWidth="1"/>
+    <col min="4" max="5" width="23.7109375" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="52" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59" t="s">
+      <c r="D2" s="53"/>
+      <c r="E2" s="53" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59" t="s">
+      <c r="D3" s="53"/>
+      <c r="E3" s="53" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="53" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59" t="s">
+      <c r="D5" s="53"/>
+      <c r="E5" s="53" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59" t="s">
+      <c r="D6" s="53"/>
+      <c r="E6" s="53" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
     </row>
     <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59" t="s">
+      <c r="D8" s="53"/>
+      <c r="E8" s="53" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59" t="s">
+      <c r="D9" s="53"/>
+      <c r="E9" s="53" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="59"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="59"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="59"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
+      <c r="A16" s="53"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="59"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="59"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
+      <c r="A18" s="53"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="59"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
+      <c r="A20" s="53"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="59"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
+      <c r="A22" s="53"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="59"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
+      <c r="A23" s="53"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="59"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
+      <c r="A24" s="53"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="59"/>
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
+      <c r="A25" s="53"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="59"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
+      <c r="A26" s="53"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="59"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
+      <c r="A27" s="53"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="59"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
+      <c r="A28" s="53"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="59"/>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
+      <c r="A29" s="53"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="59"/>
-      <c r="B30" s="59"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
+      <c r="A30" s="53"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="59"/>
-      <c r="B31" s="59"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
+      <c r="A31" s="53"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="59"/>
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
+      <c r="A32" s="53"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="59"/>
-      <c r="B33" s="59"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
+      <c r="A33" s="53"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6903,4 +6904,22 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="61.7109375" customWidth="1"/>
+    <col min="12" max="12" width="141" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>